<commit_message>
fixed json file bug
</commit_message>
<xml_diff>
--- a/Assignment-3-Data-Formats/JSON_books.xlsx
+++ b/Assignment-3-Data-Formats/JSON_books.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Category</t>
   </si>
@@ -32,19 +32,31 @@
     <t>cooking</t>
   </si>
   <si>
+    <t>Everyday Italian</t>
+  </si>
+  <si>
     <t>Giada De Laurentiis</t>
   </si>
   <si>
     <t>children</t>
   </si>
   <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
     <t>J K. Rowling</t>
   </si>
   <si>
     <t>web</t>
   </si>
   <si>
+    <t>XQuery Kick Start</t>
+  </si>
+  <si>
     <t>James McGovern, Per Bothner, Kurt Cagle, James Linn, Vaidyanathan Nagarajan</t>
+  </si>
+  <si>
+    <t>Learning XML</t>
   </si>
   <si>
     <t>Erik T. Ray</t>
@@ -101,7 +113,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.866576194763184" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.2330265045166" customWidth="1"/>
     <col min="3" max="3" width="78.29070281982422" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
@@ -129,10 +141,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0">
         <v>2005</v>
@@ -143,13 +155,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0">
         <v>2005</v>
@@ -160,13 +172,13 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0">
         <v>2003</v>
@@ -177,13 +189,13 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D5" s="0">
         <v>2003</v>

</xml_diff>